<commit_message>
Up Test Case and Bug Report XLSX
</commit_message>
<xml_diff>
--- a/TEMA 3/TAREA 2 QA. Test Case.xlsx
+++ b/TEMA 3/TAREA 2 QA. Test Case.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="108">
   <si>
     <t>ID</t>
   </si>
@@ -500,6 +500,9 @@
     </r>
   </si>
   <si>
+    <t>BR002</t>
+  </si>
+  <si>
     <t>TC004</t>
   </si>
   <si>
@@ -563,7 +566,68 @@
     </r>
   </si>
   <si>
-    <t>La sección de teoría se minimiza y la ventana del editor se expande a todo el ancho de la página. El botón se reducirá a un icono de un libro sin texto.</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">La </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>sección de teoría se minimiza</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve"> y la ventana del </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>editor se expande a todo el ancho de la página</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>El botón se reducirá a un icono</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve"> de un libro sin texto.</t>
+    </r>
+  </si>
+  <si>
+    <t>BR003</t>
   </si>
   <si>
     <r>
@@ -804,7 +868,7 @@
     <t>El editor debe permitirnos escribir el código en la línea resaltada en gris.</t>
   </si>
   <si>
-    <t>Escribir carácteres al final de las lineas del codigo de inicio que esta bloqueado.</t>
+    <t>Escribir carácteres al final de cualquiera de las lineas del codigo de inicio que esta bloqueado.</t>
   </si>
   <si>
     <t>El editor de Código debera permitirnos escribir texto al final de cada linea.</t>
@@ -813,7 +877,7 @@
     <t>TC006</t>
   </si>
   <si>
-    <t>PRUEBA DE VERIFICACION DEL CODIGO EN EL EDITOR.</t>
+    <t>PRUEBA DE VERIFICACION DEL CODIGO EN EL EDITOR CON EL BOTON COMPROBAR</t>
   </si>
   <si>
     <r>
@@ -914,6 +978,9 @@
     </r>
   </si>
   <si>
+    <t>BR004</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -953,6 +1020,9 @@
     <t>Como resultado se abre una página con la siguente pregunta a responder de la lista.</t>
   </si>
   <si>
+    <t>BR005</t>
+  </si>
+  <si>
     <t>TC007</t>
   </si>
   <si>
@@ -1214,6 +1284,9 @@
     </r>
   </si>
   <si>
+    <t>BR006</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -1265,7 +1338,7 @@
         <color theme="1"/>
         <sz val="12.0"/>
       </rPr>
-      <t>"Política de privacidad" sobre el cuál hacemos clic.</t>
+      <t>"Política de privacidad", hacemos click.</t>
     </r>
   </si>
   <si>
@@ -1296,6 +1369,9 @@
     </r>
   </si>
   <si>
+    <t>BR007</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -1329,25 +1405,20 @@
         <color theme="1"/>
         <sz val="12.0"/>
       </rPr>
-      <t xml:space="preserve">La ventana modal </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t>debera cerrarse</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t xml:space="preserve"> por completo.</t>
-    </r>
+      <t xml:space="preserve">La ventana modal debera </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>cerrarse por completo al hacer click en la "X".</t>
+    </r>
+  </si>
+  <si>
+    <t>BR008</t>
   </si>
   <si>
     <t>TC010</t>
@@ -1378,7 +1449,7 @@
         <color theme="1"/>
         <sz val="12.0"/>
       </rPr>
-      <t xml:space="preserve">Responder a cada pregunta con las respuestas proporcionadas en las pre- condiciones escribiendo en el editor de codigo, segun la numeracion de cada pregunta. y luego </t>
+      <t xml:space="preserve">Responder a cada pregunta con las respuestas proporcionadas en las pre- condiciones, escribiendo en el editor de codigo, segun la numeracion de cada pregunta. luego </t>
     </r>
     <r>
       <rPr>
@@ -1395,7 +1466,7 @@
         <color theme="1"/>
         <sz val="12.0"/>
       </rPr>
-      <t xml:space="preserve">  (El boton cambiara de texto a "Siguiente Pregunta" pulsarlo y repetir este paso siguiendo el orden de las preguntas).</t>
+      <t xml:space="preserve">  (El boton cambiara de texto a "Siguiente Pregunta" pulsarlo y repetir este paso siguiendo el orden de las preguntas y Respuestas en las pre-condiciones).</t>
     </r>
   </si>
   <si>
@@ -1418,6 +1489,9 @@
     </r>
   </si>
   <si>
+    <t>BR009</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -1441,7 +1515,7 @@
         <color rgb="FF000000"/>
         <sz val="12.0"/>
       </rPr>
-      <t xml:space="preserve"> en el editor de codigo, luego presionar el boton de color naranja "Comprobar". (Repetir este Paso pulsando las flechas en el menu de navegación)</t>
+      <t xml:space="preserve"> en el editor de codigo, luego presionar el boton de color naranja "Comprobar". (Repetir este Paso pulsando las flechas en el menu de navegación en cada pregunta hasta el final)</t>
     </r>
   </si>
   <si>
@@ -1462,6 +1536,9 @@
       </rPr>
       <t>COMPILACION INCORRECTA.</t>
     </r>
+  </si>
+  <si>
+    <t>BR0010</t>
   </si>
 </sst>
 </file>
@@ -1471,7 +1548,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1522,6 +1599,12 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1533,18 +1616,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEA9999"/>
-        <bgColor rgb="FFEA9999"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1559,7 +1636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="39">
     <border/>
     <border>
       <left style="medium">
@@ -1920,14 +1997,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
     </border>
     <border>
       <top style="thin">
@@ -1967,7 +2036,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="68">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2100,10 +2169,10 @@
     <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="34" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2112,13 +2181,10 @@
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="20" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="20" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2127,15 +2193,12 @@
     <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="20" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="34" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="35" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="36" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="36" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2144,10 +2207,10 @@
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="38" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="37" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="39" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="38" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2700,13 +2763,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -2761,27 +2824,27 @@
       <c r="A5" s="36">
         <v>2.0</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="64"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" ht="109.5" customHeight="1">
-      <c r="A6" s="65">
+      <c r="A6" s="63">
         <v>3.0</v>
       </c>
-      <c r="B6" s="66" t="s">
-        <v>93</v>
+      <c r="B6" s="64" t="s">
+        <v>100</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="67" t="s">
-        <v>94</v>
+      <c r="E6" s="65" t="s">
+        <v>101</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -2824,11 +2887,11 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C9" s="23"/>
-      <c r="D9" s="60" t="s">
-        <v>96</v>
+      <c r="D9" s="59" t="s">
+        <v>103</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="29" t="b">
@@ -2837,18 +2900,20 @@
       <c r="G9" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="61"/>
+      <c r="H9" s="32" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="10" ht="81.75" customHeight="1">
       <c r="A10" s="27">
         <v>2.0</v>
       </c>
-      <c r="B10" s="68" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="69"/>
+      <c r="B10" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="67"/>
       <c r="D10" s="28" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="29" t="b">
@@ -2857,7 +2922,9 @@
       <c r="G10" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="56"/>
+      <c r="H10" s="32" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="11" ht="18.0" customHeight="1">
       <c r="A11" s="27">
@@ -3479,7 +3546,9 @@
       <c r="G11" s="51" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="52"/>
+      <c r="H11" s="52" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="41" t="s">
@@ -3559,13 +3628,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E1" s="54"/>
       <c r="F1" s="54"/>
@@ -3667,11 +3736,11 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="29" t="b">
@@ -3687,11 +3756,11 @@
         <v>2.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="30" t="b">
@@ -3700,18 +3769,20 @@
       <c r="G9" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="56"/>
+      <c r="H9" s="32" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" ht="62.25" customHeight="1">
-      <c r="A10" s="57">
+      <c r="A10" s="56">
         <v>3.0</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="29" t="b">
@@ -3720,18 +3791,18 @@
       <c r="G10" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="58"/>
+      <c r="H10" s="57"/>
     </row>
     <row r="11" ht="66.75" customHeight="1">
-      <c r="A11" s="57">
+      <c r="A11" s="56">
         <v>4.0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="29" t="b">
@@ -3829,13 +3900,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -3937,11 +4008,11 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="29" t="b">
@@ -3957,11 +4028,11 @@
         <v>2.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="29" t="b">
@@ -3977,11 +4048,11 @@
         <v>3.0</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C10" s="23"/>
-      <c r="D10" s="59" t="s">
-        <v>60</v>
+      <c r="D10" s="58" t="s">
+        <v>62</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="29" t="b">
@@ -3997,11 +4068,11 @@
         <v>4.0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="28" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="29" t="b">
@@ -4128,13 +4199,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -4236,11 +4307,11 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C8" s="23"/>
-      <c r="D8" s="60" t="s">
-        <v>66</v>
+      <c r="D8" s="59" t="s">
+        <v>68</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="29" t="b">
@@ -4249,18 +4320,20 @@
       <c r="G8" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="61"/>
+      <c r="H8" s="32" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" ht="81.0" customHeight="1">
-      <c r="A9" s="57">
+      <c r="A9" s="56">
         <v>2.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="28" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="30" t="b">
@@ -4269,7 +4342,9 @@
       <c r="G9" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="56"/>
+      <c r="H9" s="32" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="36">
@@ -4355,13 +4430,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -4463,11 +4538,11 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C8" s="23"/>
-      <c r="D8" s="60" t="s">
-        <v>72</v>
+      <c r="D8" s="59" t="s">
+        <v>76</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="29" t="b">
@@ -4481,11 +4556,11 @@
     <row r="9" ht="81.0" customHeight="1">
       <c r="A9" s="27"/>
       <c r="B9" s="28" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="28" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="29" t="b">
@@ -4501,11 +4576,11 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="28" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="29" t="b">
@@ -4521,11 +4596,11 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="28" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="29" t="b">
@@ -4666,13 +4741,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -4774,11 +4849,11 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C8" s="23"/>
-      <c r="D8" s="60" t="s">
-        <v>82</v>
+      <c r="D8" s="59" t="s">
+        <v>86</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="29" t="b">
@@ -4787,16 +4862,18 @@
       <c r="G8" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="61"/>
+      <c r="H8" s="32" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="9" ht="81.0" customHeight="1">
       <c r="A9" s="27"/>
       <c r="B9" s="28" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="28" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="29" t="b">
@@ -4961,13 +5038,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -5069,11 +5146,11 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C8" s="23"/>
-      <c r="D8" s="60" t="s">
-        <v>88</v>
+      <c r="D8" s="59" t="s">
+        <v>93</v>
       </c>
       <c r="E8" s="23"/>
       <c r="F8" s="29" t="b">
@@ -5082,18 +5159,20 @@
       <c r="G8" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="61"/>
+      <c r="H8" s="32" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="9" ht="38.25" customHeight="1">
       <c r="A9" s="27">
         <v>2.0</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="28" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="29" t="b">
@@ -5102,7 +5181,9 @@
       <c r="G9" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="56"/>
+      <c r="H9" s="32" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="10" ht="18.0" customHeight="1">
       <c r="A10" s="27">

</xml_diff>